<commit_message>
Forrests mapped, needs names still.
</commit_message>
<xml_diff>
--- a/Planning/Forrest West.xlsx
+++ b/Planning/Forrest West.xlsx
@@ -473,7 +473,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -581,7 +581,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="4"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="2"/>
     </row>
@@ -595,7 +595,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>